<commit_message>
JTS data mods to make parallel structure for data processing code. Updated ToDo list.
</commit_message>
<xml_diff>
--- a/data/T29R09_data.xlsx
+++ b/data/T29R09_data.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kara Fox\Documents\Kara GLO\RStudio\GLO_sage\Sage_GLO\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/New Mexico/USGS/Research/Sage GLO/Sage_GLO/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F29CF28-0341-4F81-9CE0-7E1DD2B7F44E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F7767A-6D9B-394F-B225-F0A594EC6833}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
+    <workbookView xWindow="0" yWindow="1220" windowWidth="23260" windowHeight="12580" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
   </bookViews>
   <sheets>
-    <sheet name="1881" sheetId="1" r:id="rId1"/>
+    <sheet name="1880Survey" sheetId="1" r:id="rId1"/>
     <sheet name="1881notes" sheetId="2" r:id="rId2"/>
-    <sheet name="1940" sheetId="3" r:id="rId3"/>
+    <sheet name="1940Survey" sheetId="3" r:id="rId3"/>
     <sheet name="1940notes" sheetId="4" r:id="rId4"/>
+    <sheet name="1880Metadata" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -358,7 +359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="137">
   <si>
     <t>Survey_type</t>
   </si>
@@ -766,6 +767,9 @@
   </si>
   <si>
     <t xml:space="preserve">Land valuable for grazing and show effects of having been overgrazed by sheep. </t>
+  </si>
+  <si>
+    <t>Actually surveyed in 1881; tab reads 1880 for consistency in the data processing R script</t>
   </si>
 </sst>
 </file>
@@ -1179,23 +1183,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5C64BF-EBB4-4133-9976-AA11B41391F4}">
   <dimension ref="A1:AD40"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="3.5546875" customWidth="1"/>
+    <col min="1" max="1" width="15.83203125" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="6" max="6" width="3.5" customWidth="1"/>
     <col min="9" max="9" width="60.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.21875" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1269,7 +1273,7 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1298,9 +1302,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
       </c>
       <c r="C3" t="s">
         <v>27</v>
@@ -1324,9 +1331,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
       </c>
       <c r="C4" t="s">
         <v>28</v>
@@ -1350,9 +1360,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -1376,9 +1389,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>30</v>
@@ -1402,9 +1418,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>31</v>
@@ -1428,9 +1447,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>32</v>
@@ -1454,9 +1476,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>25</v>
       </c>
       <c r="C9" t="s">
         <v>33</v>
@@ -1480,9 +1505,12 @@
         <v>80</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>25</v>
       </c>
       <c r="C10" t="s">
         <v>62</v>
@@ -1497,9 +1525,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
       </c>
       <c r="C11" t="s">
         <v>34</v>
@@ -1523,9 +1554,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>35</v>
@@ -1549,9 +1583,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
       </c>
       <c r="C13" t="s">
         <v>72</v>
@@ -1575,9 +1612,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>25</v>
       </c>
       <c r="C14" t="s">
         <v>36</v>
@@ -1601,9 +1641,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>25</v>
       </c>
       <c r="C15" t="s">
         <v>37</v>
@@ -1627,9 +1670,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>25</v>
       </c>
       <c r="C16" t="s">
         <v>38</v>
@@ -1653,9 +1699,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>39</v>
@@ -1679,9 +1728,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>25</v>
       </c>
       <c r="C18" t="s">
         <v>40</v>
@@ -1705,9 +1757,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>25</v>
       </c>
       <c r="C19" t="s">
         <v>41</v>
@@ -1731,9 +1786,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>25</v>
       </c>
       <c r="C20" t="s">
         <v>42</v>
@@ -1757,9 +1815,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>43</v>
@@ -1783,9 +1844,12 @@
         <v>90</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
       </c>
       <c r="C22" t="s">
         <v>44</v>
@@ -1809,9 +1873,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>25</v>
       </c>
       <c r="C23" t="s">
         <v>45</v>
@@ -1835,9 +1902,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>25</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -1861,9 +1931,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>46</v>
@@ -1887,9 +1960,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
       </c>
       <c r="C26" t="s">
         <v>48</v>
@@ -1913,9 +1989,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>25</v>
       </c>
       <c r="C27" t="s">
         <v>49</v>
@@ -1939,9 +2018,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>25</v>
       </c>
       <c r="C28" t="s">
         <v>50</v>
@@ -1965,9 +2047,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>25</v>
       </c>
       <c r="C29" t="s">
         <v>51</v>
@@ -1991,9 +2076,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>22</v>
+      </c>
+      <c r="B30" t="s">
+        <v>25</v>
       </c>
       <c r="C30" t="s">
         <v>52</v>
@@ -2017,9 +2105,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
+      </c>
+      <c r="B31" t="s">
+        <v>25</v>
       </c>
       <c r="C31" t="s">
         <v>53</v>
@@ -2043,9 +2134,12 @@
         <v>99</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
+      </c>
+      <c r="B32" t="s">
+        <v>25</v>
       </c>
       <c r="C32" t="s">
         <v>54</v>
@@ -2069,9 +2163,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
+      </c>
+      <c r="B33" t="s">
+        <v>25</v>
       </c>
       <c r="C33" t="s">
         <v>55</v>
@@ -2095,9 +2192,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>25</v>
       </c>
       <c r="C34" t="s">
         <v>56</v>
@@ -2121,9 +2221,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>22</v>
+      </c>
+      <c r="B35" t="s">
+        <v>25</v>
       </c>
       <c r="C35" t="s">
         <v>57</v>
@@ -2147,9 +2250,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>22</v>
+      </c>
+      <c r="B36" t="s">
+        <v>25</v>
       </c>
       <c r="C36" t="s">
         <v>60</v>
@@ -2173,9 +2279,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>22</v>
+      </c>
+      <c r="B37" t="s">
+        <v>25</v>
       </c>
       <c r="C37" t="s">
         <v>58</v>
@@ -2199,9 +2308,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>22</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
       </c>
       <c r="C38" t="s">
         <v>103</v>
@@ -2225,9 +2337,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>22</v>
+      </c>
+      <c r="B39" t="s">
+        <v>25</v>
       </c>
       <c r="C39" t="s">
         <v>59</v>
@@ -2251,9 +2366,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>22</v>
+      </c>
+      <c r="B40" t="s">
+        <v>25</v>
       </c>
       <c r="C40" t="s">
         <v>61</v>
@@ -2297,12 +2415,12 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="108.109375" customWidth="1"/>
+    <col min="1" max="1" width="108.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -2316,24 +2434,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B3FAA3-4E86-4E5F-9736-210B302B7A32}">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A18" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="6" max="6" width="3.77734375" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" customWidth="1"/>
     <col min="9" max="9" width="70.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" customWidth="1"/>
+    <col min="10" max="10" width="12.5" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.109375" customWidth="1"/>
+    <col min="12" max="12" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2407,7 +2525,7 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -2436,7 +2554,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -2465,7 +2583,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -2494,7 +2612,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -2523,7 +2641,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -2552,7 +2670,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -2581,7 +2699,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -2610,7 +2728,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -2639,7 +2757,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -2668,7 +2786,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -2697,7 +2815,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -2726,7 +2844,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -2755,7 +2873,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -2784,7 +2902,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -2813,7 +2931,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -2842,7 +2960,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -2871,7 +2989,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -2900,7 +3018,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -2929,7 +3047,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -2958,7 +3076,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -2987,7 +3105,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -3016,7 +3134,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -3045,7 +3163,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -3074,7 +3192,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -3103,7 +3221,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -3132,7 +3250,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -3161,7 +3279,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -3190,7 +3308,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -3235,23 +3353,43 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1634017A-8458-4693-8385-F8087CEF47D0}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="119.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>135</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74E99880-3DFF-484B-8368-48CD6B574AF1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating data sheets to correspond with each sheet. Creating new data sheets as needed.
</commit_message>
<xml_diff>
--- a/data/T29R09_data.xlsx
+++ b/data/T29R09_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jtstevens/Documents/New Mexico/USGS/Research/Sage GLO/Sage_GLO/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kara Fox\Documents\Kara GLO\RStudio\GLO_sage\Sage_GLO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6F7767A-6D9B-394F-B225-F0A594EC6833}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0916777D-739D-4759-9661-7E5BF2635967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1220" windowWidth="23260" windowHeight="12580" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
+    <workbookView xWindow="-28920" yWindow="-5295" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
   </bookViews>
   <sheets>
     <sheet name="1880Survey" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="133">
   <si>
     <t>Survey_type</t>
   </si>
@@ -454,15 +454,6 @@
     <t>30-09-35-S</t>
   </si>
   <si>
-    <t>30-09-34-S</t>
-  </si>
-  <si>
-    <t>30-09-33-S</t>
-  </si>
-  <si>
-    <t>30-09-32-S</t>
-  </si>
-  <si>
     <t>29-09-36-W</t>
   </si>
   <si>
@@ -599,9 +590,6 @@
   </si>
   <si>
     <t>Land rolling, bunch and gramma grass</t>
-  </si>
-  <si>
-    <t>August 21 1881</t>
   </si>
   <si>
     <t>Land 30 chn rolling prarie between mountainous. Pinon and cedar timber. Bunch and gramma grass</t>
@@ -1181,25 +1169,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5C64BF-EBB4-4133-9976-AA11B41391F4}">
-  <dimension ref="A1:AD40"/>
+  <dimension ref="A1:AD35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35:XFD39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" customWidth="1"/>
-    <col min="2" max="2" width="12.1640625" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
-    <col min="6" max="6" width="3.5" customWidth="1"/>
+    <col min="1" max="1" width="15.77734375" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+    <col min="3" max="3" width="14.77734375" customWidth="1"/>
+    <col min="6" max="6" width="3.44140625" customWidth="1"/>
     <col min="9" max="9" width="60.33203125" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" customWidth="1"/>
+    <col min="10" max="10" width="12.109375" customWidth="1"/>
     <col min="11" max="11" width="18" customWidth="1"/>
     <col min="12" max="12" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1273,7 +1261,7 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1281,19 +1269,19 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G2" t="s">
         <v>75</v>
       </c>
       <c r="I2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
@@ -1302,7 +1290,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1310,28 +1298,28 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
         <v>75</v>
       </c>
       <c r="I3" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1339,19 +1327,19 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I4" t="s">
-        <v>76</v>
+        <v>98</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1360,7 +1348,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1368,19 +1356,19 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G5" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1389,7 +1377,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1397,19 +1385,19 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G6" t="s">
         <v>75</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
@@ -1418,7 +1406,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1426,19 +1414,19 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G7" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I7" t="s">
-        <v>79</v>
+        <v>100</v>
       </c>
       <c r="J7" t="s">
         <v>23</v>
@@ -1447,7 +1435,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1455,19 +1443,19 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G8" t="s">
         <v>75</v>
       </c>
       <c r="I8" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="J8" t="s">
         <v>23</v>
@@ -1476,7 +1464,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1484,28 +1472,28 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>52</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G9" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I9" t="s">
-        <v>77</v>
+        <v>97</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
       </c>
       <c r="L9" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1513,10 +1501,19 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>62</v>
+        <v>99</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" t="s">
+        <v>76</v>
       </c>
       <c r="J10" t="s">
         <v>23</v>
@@ -1525,7 +1522,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1533,19 +1530,19 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I11" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
       <c r="J11" t="s">
         <v>23</v>
@@ -1554,7 +1551,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1562,19 +1559,19 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>53</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
@@ -1583,7 +1580,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1591,13 +1588,13 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G13" t="s">
         <v>75</v>
@@ -1612,7 +1609,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1620,16 +1617,16 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G14" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="I14" t="s">
         <v>83</v>
@@ -1641,7 +1638,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1649,19 +1646,19 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G15" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I15" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="J15" t="s">
         <v>23</v>
@@ -1670,7 +1667,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1678,19 +1675,19 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G16" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I16" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="J16" t="s">
         <v>23</v>
@@ -1699,7 +1696,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1707,19 +1704,19 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G17" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I17" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
@@ -1728,7 +1725,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1736,28 +1733,28 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G18" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="I18" t="s">
-        <v>86</v>
+        <v>93</v>
       </c>
       <c r="J18" t="s">
         <v>23</v>
       </c>
       <c r="L18" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1765,19 +1762,19 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G19" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="I19" t="s">
-        <v>87</v>
+        <v>92</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
@@ -1786,7 +1783,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1794,19 +1791,19 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G20" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I20" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
@@ -1815,7 +1812,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1823,16 +1820,16 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="G21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I21" t="s">
         <v>89</v>
@@ -1841,30 +1838,30 @@
         <v>23</v>
       </c>
       <c r="L21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>25</v>
+      </c>
+      <c r="C22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>71</v>
+      </c>
+      <c r="G22" t="s">
+        <v>75</v>
+      </c>
+      <c r="I22" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>25</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>74</v>
-      </c>
-      <c r="G22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I22" t="s">
-        <v>91</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
@@ -1873,7 +1870,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1881,19 +1878,19 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G23" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I23" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
@@ -1902,7 +1899,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1910,19 +1907,19 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
         <v>75</v>
       </c>
       <c r="I24" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
@@ -1931,7 +1928,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1939,19 +1936,19 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>46</v>
+        <v>32</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G25" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I25" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
@@ -1960,7 +1957,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1968,19 +1965,19 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>48</v>
+        <v>69</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="G26" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I26" t="s">
-        <v>93</v>
+        <v>78</v>
       </c>
       <c r="J26" t="s">
         <v>23</v>
@@ -1989,7 +1986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -1997,19 +1994,19 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G27" t="s">
         <v>75</v>
       </c>
       <c r="I27" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="J27" t="s">
         <v>23</v>
@@ -2018,7 +2015,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2026,19 +2023,19 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G28" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I28" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="J28" t="s">
         <v>23</v>
@@ -2047,7 +2044,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2055,19 +2052,19 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="D29" t="s">
         <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G29" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I29" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="J29" t="s">
         <v>23</v>
@@ -2076,7 +2073,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2084,19 +2081,19 @@
         <v>25</v>
       </c>
       <c r="C30" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="D30" t="s">
         <v>21</v>
       </c>
       <c r="E30" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I30" t="s">
-        <v>96</v>
+        <v>73</v>
       </c>
       <c r="J30" t="s">
         <v>23</v>
@@ -2105,7 +2102,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2113,28 +2110,28 @@
         <v>25</v>
       </c>
       <c r="C31" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="D31" t="s">
         <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G31" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="I31" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="J31" t="s">
         <v>23</v>
       </c>
       <c r="L31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2142,19 +2139,19 @@
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G32" t="s">
         <v>75</v>
       </c>
       <c r="I32" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="J32" t="s">
         <v>23</v>
@@ -2163,7 +2160,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2171,19 +2168,19 @@
         <v>25</v>
       </c>
       <c r="C33" t="s">
-        <v>55</v>
+        <v>26</v>
       </c>
       <c r="D33" t="s">
         <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G33" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I33" t="s">
-        <v>101</v>
+        <v>70</v>
       </c>
       <c r="J33" t="s">
         <v>23</v>
@@ -2192,7 +2189,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2200,19 +2197,19 @@
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="D34" t="s">
         <v>21</v>
       </c>
       <c r="E34" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G34" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="I34" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="J34" t="s">
         <v>23</v>
@@ -2221,7 +2218,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2229,19 +2226,10 @@
         <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="D35" t="s">
         <v>21</v>
-      </c>
-      <c r="E35" t="s">
-        <v>74</v>
-      </c>
-      <c r="G35" t="s">
-        <v>75</v>
-      </c>
-      <c r="I35" t="s">
-        <v>102</v>
       </c>
       <c r="J35" t="s">
         <v>23</v>
@@ -2250,152 +2238,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>22</v>
-      </c>
-      <c r="B36" t="s">
-        <v>25</v>
-      </c>
-      <c r="C36" t="s">
-        <v>60</v>
-      </c>
-      <c r="D36" t="s">
-        <v>21</v>
-      </c>
-      <c r="E36" t="s">
-        <v>74</v>
-      </c>
-      <c r="G36" t="s">
-        <v>75</v>
-      </c>
-      <c r="I36" t="s">
-        <v>79</v>
-      </c>
-      <c r="J36" t="s">
-        <v>23</v>
-      </c>
-      <c r="L36" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" t="s">
-        <v>25</v>
-      </c>
-      <c r="C37" t="s">
-        <v>58</v>
-      </c>
-      <c r="D37" t="s">
-        <v>21</v>
-      </c>
-      <c r="E37" t="s">
-        <v>74</v>
-      </c>
-      <c r="G37" t="s">
-        <v>78</v>
-      </c>
-      <c r="I37" t="s">
-        <v>77</v>
-      </c>
-      <c r="J37" t="s">
-        <v>23</v>
-      </c>
-      <c r="L37" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>22</v>
-      </c>
-      <c r="B38" t="s">
-        <v>25</v>
-      </c>
-      <c r="C38" t="s">
-        <v>103</v>
-      </c>
-      <c r="D38" t="s">
-        <v>21</v>
-      </c>
-      <c r="E38" t="s">
-        <v>74</v>
-      </c>
-      <c r="G38" t="s">
-        <v>75</v>
-      </c>
-      <c r="I38" t="s">
-        <v>79</v>
-      </c>
-      <c r="J38" t="s">
-        <v>23</v>
-      </c>
-      <c r="L38" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>22</v>
-      </c>
-      <c r="B39" t="s">
-        <v>25</v>
-      </c>
-      <c r="C39" t="s">
-        <v>59</v>
-      </c>
-      <c r="D39" t="s">
-        <v>21</v>
-      </c>
-      <c r="E39" t="s">
-        <v>74</v>
-      </c>
-      <c r="G39" t="s">
-        <v>75</v>
-      </c>
-      <c r="I39" t="s">
-        <v>104</v>
-      </c>
-      <c r="J39" t="s">
-        <v>23</v>
-      </c>
-      <c r="L39" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>22</v>
-      </c>
-      <c r="B40" t="s">
-        <v>25</v>
-      </c>
-      <c r="C40" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" t="s">
-        <v>21</v>
-      </c>
-      <c r="E40" t="s">
-        <v>74</v>
-      </c>
-      <c r="G40" t="s">
-        <v>78</v>
-      </c>
-      <c r="I40" t="s">
-        <v>105</v>
-      </c>
-      <c r="J40" t="s">
-        <v>23</v>
-      </c>
-      <c r="L40" t="s">
-        <v>24</v>
-      </c>
-    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U35">
+    <sortCondition ref="C1"/>
+  </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="D1">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
@@ -2415,14 +2261,14 @@
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="108.1640625" customWidth="1"/>
+    <col min="1" max="1" width="108.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2434,24 +2280,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B3FAA3-4E86-4E5F-9736-210B302B7A32}">
   <dimension ref="A1:AD29"/>
   <sheetViews>
-    <sheetView topLeftCell="A18" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="2" max="2" width="10.33203125" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
     <col min="4" max="4" width="7" customWidth="1"/>
-    <col min="6" max="6" width="3.83203125" customWidth="1"/>
+    <col min="6" max="6" width="3.77734375" customWidth="1"/>
     <col min="9" max="9" width="70.6640625" customWidth="1"/>
-    <col min="10" max="10" width="12.5" customWidth="1"/>
+    <col min="10" max="10" width="12.44140625" customWidth="1"/>
     <col min="11" max="11" width="18.6640625" customWidth="1"/>
-    <col min="12" max="12" width="23.1640625" customWidth="1"/>
+    <col min="12" max="12" width="23.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2525,12 +2371,12 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C2" t="s">
         <v>27</v>
@@ -2539,27 +2385,27 @@
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G2" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I2" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="J2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
       <c r="B3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>26</v>
@@ -2568,201 +2414,201 @@
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G3" t="s">
+        <v>104</v>
+      </c>
+      <c r="I3" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" t="s">
+        <v>61</v>
+      </c>
+      <c r="L3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" t="s">
+        <v>63</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" t="s">
+        <v>104</v>
+      </c>
+      <c r="I4" t="s">
+        <v>106</v>
+      </c>
+      <c r="J4" t="s">
+        <v>61</v>
+      </c>
+      <c r="L4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" t="s">
+        <v>107</v>
+      </c>
+      <c r="J5" t="s">
+        <v>61</v>
+      </c>
+      <c r="L5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>60</v>
+      </c>
+      <c r="C6" t="s">
+        <v>65</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>72</v>
+      </c>
+      <c r="G6" t="s">
+        <v>104</v>
+      </c>
+      <c r="I6" t="s">
         <v>108</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J6" t="s">
+        <v>61</v>
+      </c>
+      <c r="L6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="G7" t="s">
+        <v>104</v>
+      </c>
+      <c r="I7" t="s">
         <v>109</v>
       </c>
-      <c r="J3" t="s">
-        <v>64</v>
-      </c>
-      <c r="L3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>75</v>
-      </c>
-      <c r="G4" t="s">
-        <v>108</v>
-      </c>
-      <c r="I4" t="s">
+      <c r="J7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>60</v>
+      </c>
+      <c r="C8" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>72</v>
+      </c>
+      <c r="G8" t="s">
+        <v>104</v>
+      </c>
+      <c r="I8" t="s">
         <v>110</v>
       </c>
-      <c r="J4" t="s">
-        <v>64</v>
-      </c>
-      <c r="L4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" t="s">
-        <v>108</v>
-      </c>
-      <c r="I5" t="s">
+      <c r="J8" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>60</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>72</v>
+      </c>
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+      <c r="I9" t="s">
         <v>111</v>
       </c>
-      <c r="J5" t="s">
-        <v>64</v>
-      </c>
-      <c r="L5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" t="s">
-        <v>68</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>75</v>
-      </c>
-      <c r="G6" t="s">
-        <v>108</v>
-      </c>
-      <c r="I6" t="s">
-        <v>112</v>
-      </c>
-      <c r="J6" t="s">
-        <v>64</v>
-      </c>
-      <c r="L6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B7" t="s">
-        <v>63</v>
-      </c>
-      <c r="C7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" t="s">
-        <v>108</v>
-      </c>
-      <c r="I7" t="s">
-        <v>113</v>
-      </c>
-      <c r="J7" t="s">
-        <v>64</v>
-      </c>
-      <c r="L7" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" t="s">
-        <v>63</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>75</v>
-      </c>
-      <c r="G8" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" t="s">
-        <v>114</v>
-      </c>
-      <c r="J8" t="s">
-        <v>64</v>
-      </c>
-      <c r="L8" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B9" t="s">
-        <v>63</v>
-      </c>
-      <c r="C9" t="s">
-        <v>71</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>75</v>
-      </c>
-      <c r="G9" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" t="s">
-        <v>115</v>
-      </c>
       <c r="J9" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L9" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>22</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
         <v>29</v>
@@ -2771,27 +2617,27 @@
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="J10" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>22</v>
       </c>
       <c r="B11" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C11" t="s">
         <v>30</v>
@@ -2800,541 +2646,541 @@
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I11" t="s">
+        <v>112</v>
+      </c>
+      <c r="J11" t="s">
+        <v>61</v>
+      </c>
+      <c r="L11" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="s">
+        <v>60</v>
+      </c>
+      <c r="C12" t="s">
+        <v>53</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>72</v>
+      </c>
+      <c r="G12" t="s">
+        <v>104</v>
+      </c>
+      <c r="I12" t="s">
+        <v>113</v>
+      </c>
+      <c r="J12" t="s">
+        <v>61</v>
+      </c>
+      <c r="L12" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>22</v>
+      </c>
+      <c r="B13" t="s">
+        <v>60</v>
+      </c>
+      <c r="C13" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" t="s">
+        <v>104</v>
+      </c>
+      <c r="I13" t="s">
+        <v>114</v>
+      </c>
+      <c r="J13" t="s">
+        <v>61</v>
+      </c>
+      <c r="L13" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" t="s">
+        <v>72</v>
+      </c>
+      <c r="G14" t="s">
+        <v>104</v>
+      </c>
+      <c r="I14" t="s">
+        <v>115</v>
+      </c>
+      <c r="J14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L14" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G15" t="s">
+        <v>104</v>
+      </c>
+      <c r="I15" t="s">
         <v>116</v>
       </c>
-      <c r="J11" t="s">
-        <v>64</v>
-      </c>
-      <c r="L11" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>22</v>
-      </c>
-      <c r="B12" t="s">
-        <v>63</v>
-      </c>
-      <c r="C12" t="s">
-        <v>56</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G12" t="s">
-        <v>108</v>
-      </c>
-      <c r="I12" t="s">
+      <c r="J15" t="s">
+        <v>61</v>
+      </c>
+      <c r="L15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B16" t="s">
+        <v>60</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>72</v>
+      </c>
+      <c r="G16" t="s">
+        <v>104</v>
+      </c>
+      <c r="I16" t="s">
         <v>117</v>
       </c>
-      <c r="J12" t="s">
-        <v>64</v>
-      </c>
-      <c r="L12" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B13" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" t="s">
+      <c r="J16" t="s">
+        <v>61</v>
+      </c>
+      <c r="L16" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
         <v>60</v>
       </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>75</v>
-      </c>
-      <c r="G13" t="s">
-        <v>108</v>
-      </c>
-      <c r="I13" t="s">
+      <c r="C17" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>72</v>
+      </c>
+      <c r="G17" t="s">
+        <v>104</v>
+      </c>
+      <c r="I17" t="s">
         <v>118</v>
       </c>
-      <c r="J13" t="s">
-        <v>64</v>
-      </c>
-      <c r="L13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C14" t="s">
+      <c r="J17" t="s">
+        <v>61</v>
+      </c>
+      <c r="L17" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>60</v>
+      </c>
+      <c r="C18" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>72</v>
+      </c>
+      <c r="G18" t="s">
+        <v>104</v>
+      </c>
+      <c r="I18" t="s">
+        <v>119</v>
+      </c>
+      <c r="J18" t="s">
+        <v>61</v>
+      </c>
+      <c r="L18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>72</v>
+      </c>
+      <c r="G19" t="s">
+        <v>104</v>
+      </c>
+      <c r="I19" t="s">
+        <v>120</v>
+      </c>
+      <c r="J19" t="s">
+        <v>61</v>
+      </c>
+      <c r="L19" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+      <c r="C20" t="s">
         <v>34</v>
       </c>
-      <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>75</v>
-      </c>
-      <c r="G14" t="s">
-        <v>108</v>
-      </c>
-      <c r="I14" t="s">
-        <v>119</v>
-      </c>
-      <c r="J14" t="s">
-        <v>64</v>
-      </c>
-      <c r="L14" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>72</v>
+      </c>
+      <c r="G20" t="s">
+        <v>104</v>
+      </c>
+      <c r="I20" t="s">
+        <v>121</v>
+      </c>
+      <c r="J20" t="s">
+        <v>61</v>
+      </c>
+      <c r="L20" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
         <v>35</v>
       </c>
-      <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>75</v>
-      </c>
-      <c r="G15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I15" t="s">
-        <v>120</v>
-      </c>
-      <c r="J15" t="s">
-        <v>64</v>
-      </c>
-      <c r="L15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" t="s">
-        <v>63</v>
-      </c>
-      <c r="C16" t="s">
-        <v>45</v>
-      </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" t="s">
-        <v>108</v>
-      </c>
-      <c r="I16" t="s">
-        <v>121</v>
-      </c>
-      <c r="J16" t="s">
-        <v>64</v>
-      </c>
-      <c r="L16" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" t="s">
-        <v>63</v>
-      </c>
-      <c r="C17" t="s">
-        <v>72</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" t="s">
-        <v>108</v>
-      </c>
-      <c r="I17" t="s">
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>72</v>
+      </c>
+      <c r="G21" t="s">
+        <v>104</v>
+      </c>
+      <c r="I21" t="s">
         <v>122</v>
       </c>
-      <c r="J17" t="s">
-        <v>64</v>
-      </c>
-      <c r="L17" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="J21" t="s">
+        <v>61</v>
+      </c>
+      <c r="L21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>60</v>
+      </c>
+      <c r="C22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>72</v>
+      </c>
+      <c r="G22" t="s">
+        <v>104</v>
+      </c>
+      <c r="I22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J22" t="s">
+        <v>61</v>
+      </c>
+      <c r="L22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>60</v>
+      </c>
+      <c r="C23" t="s">
         <v>36</v>
       </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" t="s">
-        <v>108</v>
-      </c>
-      <c r="I18" t="s">
-        <v>123</v>
-      </c>
-      <c r="J18" t="s">
-        <v>64</v>
-      </c>
-      <c r="L18" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>22</v>
-      </c>
-      <c r="B19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" t="s">
-        <v>48</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" t="s">
-        <v>108</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>72</v>
+      </c>
+      <c r="G23" t="s">
+        <v>104</v>
+      </c>
+      <c r="I23" t="s">
         <v>124</v>
       </c>
-      <c r="J19" t="s">
-        <v>64</v>
-      </c>
-      <c r="L19" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="J23" t="s">
+        <v>61</v>
+      </c>
+      <c r="L23" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" t="s">
         <v>37</v>
       </c>
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>75</v>
-      </c>
-      <c r="G20" t="s">
-        <v>108</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>72</v>
+      </c>
+      <c r="G24" t="s">
+        <v>104</v>
+      </c>
+      <c r="I24" t="s">
         <v>125</v>
       </c>
-      <c r="J20" t="s">
-        <v>64</v>
-      </c>
-      <c r="L20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>22</v>
-      </c>
-      <c r="B21" t="s">
-        <v>63</v>
-      </c>
-      <c r="C21" t="s">
+      <c r="J24" t="s">
+        <v>61</v>
+      </c>
+      <c r="L24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>60</v>
+      </c>
+      <c r="C25" t="s">
+        <v>51</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>72</v>
+      </c>
+      <c r="G25" t="s">
+        <v>104</v>
+      </c>
+      <c r="I25" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" t="s">
+        <v>61</v>
+      </c>
+      <c r="L25" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" t="s">
         <v>38</v>
       </c>
-      <c r="D21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" t="s">
-        <v>108</v>
-      </c>
-      <c r="I21" t="s">
-        <v>126</v>
-      </c>
-      <c r="J21" t="s">
-        <v>64</v>
-      </c>
-      <c r="L21" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
-        <v>63</v>
-      </c>
-      <c r="C22" t="s">
-        <v>51</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>75</v>
-      </c>
-      <c r="G22" t="s">
-        <v>108</v>
-      </c>
-      <c r="I22" t="s">
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>72</v>
+      </c>
+      <c r="G26" t="s">
+        <v>104</v>
+      </c>
+      <c r="I26" t="s">
+        <v>124</v>
+      </c>
+      <c r="J26" t="s">
+        <v>61</v>
+      </c>
+      <c r="L26" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>60</v>
+      </c>
+      <c r="C27" t="s">
+        <v>39</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>72</v>
+      </c>
+      <c r="G27" t="s">
+        <v>104</v>
+      </c>
+      <c r="I27" t="s">
         <v>127</v>
       </c>
-      <c r="J22" t="s">
-        <v>64</v>
-      </c>
-      <c r="L22" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>22</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
-        <v>39</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>75</v>
-      </c>
-      <c r="G23" t="s">
-        <v>108</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="J27" t="s">
+        <v>61</v>
+      </c>
+      <c r="L27" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C28" t="s">
+        <v>54</v>
+      </c>
+      <c r="D28" t="s">
+        <v>21</v>
+      </c>
+      <c r="E28" t="s">
+        <v>72</v>
+      </c>
+      <c r="G28" t="s">
+        <v>104</v>
+      </c>
+      <c r="I28" t="s">
         <v>128</v>
       </c>
-      <c r="J23" t="s">
-        <v>64</v>
-      </c>
-      <c r="L23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>22</v>
-      </c>
-      <c r="B24" t="s">
-        <v>63</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="J28" t="s">
+        <v>61</v>
+      </c>
+      <c r="L28" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" t="s">
         <v>40</v>
       </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>75</v>
-      </c>
-      <c r="G24" t="s">
-        <v>108</v>
-      </c>
-      <c r="I24" t="s">
+      <c r="D29" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" t="s">
+        <v>72</v>
+      </c>
+      <c r="G29" t="s">
+        <v>104</v>
+      </c>
+      <c r="I29" t="s">
         <v>129</v>
       </c>
-      <c r="J24" t="s">
-        <v>64</v>
-      </c>
-      <c r="L24" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>22</v>
-      </c>
-      <c r="B25" t="s">
-        <v>63</v>
-      </c>
-      <c r="C25" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>75</v>
-      </c>
-      <c r="G25" t="s">
-        <v>108</v>
-      </c>
-      <c r="I25" t="s">
-        <v>130</v>
-      </c>
-      <c r="J25" t="s">
-        <v>64</v>
-      </c>
-      <c r="L25" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>22</v>
-      </c>
-      <c r="B26" t="s">
-        <v>63</v>
-      </c>
-      <c r="C26" t="s">
-        <v>41</v>
-      </c>
-      <c r="D26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" t="s">
-        <v>128</v>
-      </c>
-      <c r="J26" t="s">
-        <v>64</v>
-      </c>
-      <c r="L26" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>22</v>
-      </c>
-      <c r="B27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C27" t="s">
-        <v>42</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" t="s">
-        <v>108</v>
-      </c>
-      <c r="I27" t="s">
-        <v>131</v>
-      </c>
-      <c r="J27" t="s">
-        <v>64</v>
-      </c>
-      <c r="L27" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>63</v>
-      </c>
-      <c r="C28" t="s">
-        <v>57</v>
-      </c>
-      <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" t="s">
-        <v>108</v>
-      </c>
-      <c r="I28" t="s">
-        <v>132</v>
-      </c>
-      <c r="J28" t="s">
-        <v>64</v>
-      </c>
-      <c r="L28" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" t="s">
-        <v>75</v>
-      </c>
-      <c r="G29" t="s">
-        <v>108</v>
-      </c>
-      <c r="I29" t="s">
-        <v>133</v>
-      </c>
       <c r="J29" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="L29" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -3357,19 +3203,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="119.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -3385,11 +3231,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixing issues with T29R09 and T30R09 1940 data
</commit_message>
<xml_diff>
--- a/data/T29R09_data.xlsx
+++ b/data/T29R09_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kara Fox\Documents\Kara GLO\RStudio\GLO_sage\Sage_GLO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0916777D-739D-4759-9661-7E5BF2635967}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE55E6C-68D4-42F4-9A0F-B57E6920D07F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-5295" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
   </bookViews>
   <sheets>
     <sheet name="1880Survey" sheetId="1" r:id="rId1"/>
@@ -359,7 +359,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="130">
   <si>
     <t>Survey_type</t>
   </si>
@@ -448,12 +448,6 @@
     <t>29-09-34-S</t>
   </si>
   <si>
-    <t>30-09-36-S</t>
-  </si>
-  <si>
-    <t>30-09-35-S</t>
-  </si>
-  <si>
     <t>29-09-36-W</t>
   </si>
   <si>
@@ -695,9 +689,6 @@
   </si>
   <si>
     <t xml:space="preserve">Land rolling and hilly. Timber, pinon and scrub cedar. Undergrowth, sage. </t>
-  </si>
-  <si>
-    <t>Land, level and rolling. Timber sparse pinon and scrub cedar. Undergrowth, sage.</t>
   </si>
   <si>
     <t xml:space="preserve">Land rolling. Timber, none. Undergrowth, sage up to 3 ft high. </t>
@@ -1269,19 +1260,19 @@
         <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2" t="s">
         <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="J2" t="s">
         <v>23</v>
@@ -1298,25 +1289,25 @@
         <v>25</v>
       </c>
       <c r="C3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D3" t="s">
         <v>21</v>
       </c>
       <c r="E3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="J3" t="s">
         <v>23</v>
       </c>
       <c r="L3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
@@ -1327,19 +1318,19 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
       </c>
       <c r="E4" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I4" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="J4" t="s">
         <v>23</v>
@@ -1356,19 +1347,19 @@
         <v>25</v>
       </c>
       <c r="C5" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D5" t="s">
         <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G5" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J5" t="s">
         <v>23</v>
@@ -1385,19 +1376,19 @@
         <v>25</v>
       </c>
       <c r="C6" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="D6" t="s">
         <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="J6" t="s">
         <v>23</v>
@@ -1414,19 +1405,19 @@
         <v>25</v>
       </c>
       <c r="C7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
         <v>21</v>
       </c>
       <c r="E7" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I7" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="J7" t="s">
         <v>23</v>
@@ -1443,19 +1434,19 @@
         <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D8" t="s">
         <v>21</v>
       </c>
       <c r="E8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I8" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J8" t="s">
         <v>23</v>
@@ -1472,19 +1463,19 @@
         <v>25</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" t="s">
         <v>21</v>
       </c>
       <c r="E9" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
@@ -1501,19 +1492,19 @@
         <v>25</v>
       </c>
       <c r="C10" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D10" t="s">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G10" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I10" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J10" t="s">
         <v>23</v>
@@ -1530,19 +1521,19 @@
         <v>25</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
         <v>21</v>
       </c>
       <c r="E11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="J11" t="s">
         <v>23</v>
@@ -1559,19 +1550,19 @@
         <v>25</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D12" t="s">
         <v>21</v>
       </c>
       <c r="E12" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I12" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
@@ -1588,19 +1579,19 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" t="s">
         <v>21</v>
       </c>
       <c r="E13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I13" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J13" t="s">
         <v>23</v>
@@ -1617,19 +1608,19 @@
         <v>25</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D14" t="s">
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="J14" t="s">
         <v>23</v>
@@ -1646,19 +1637,19 @@
         <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D15" t="s">
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I15" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="J15" t="s">
         <v>23</v>
@@ -1675,19 +1666,19 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D16" t="s">
         <v>21</v>
       </c>
       <c r="E16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G16" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I16" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="J16" t="s">
         <v>23</v>
@@ -1704,19 +1695,19 @@
         <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D17" t="s">
         <v>21</v>
       </c>
       <c r="E17" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G17" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J17" t="s">
         <v>23</v>
@@ -1733,25 +1724,25 @@
         <v>25</v>
       </c>
       <c r="C18" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D18" t="s">
         <v>21</v>
       </c>
       <c r="E18" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="I18" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="L18" t="s">
         <v>93</v>
-      </c>
-      <c r="J18" t="s">
-        <v>23</v>
-      </c>
-      <c r="L18" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -1762,19 +1753,19 @@
         <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D19" t="s">
         <v>21</v>
       </c>
       <c r="E19" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G19" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I19" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="J19" t="s">
         <v>23</v>
@@ -1791,19 +1782,19 @@
         <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D20" t="s">
         <v>21</v>
       </c>
       <c r="E20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G20" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J20" t="s">
         <v>23</v>
@@ -1820,19 +1811,19 @@
         <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D21" t="s">
         <v>21</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G21" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I21" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="J21" t="s">
         <v>23</v>
@@ -1849,19 +1840,19 @@
         <v>25</v>
       </c>
       <c r="C22" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D22" t="s">
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G22" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I22" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="J22" t="s">
         <v>23</v>
@@ -1878,19 +1869,19 @@
         <v>25</v>
       </c>
       <c r="C23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D23" t="s">
         <v>21</v>
       </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G23" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I23" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J23" t="s">
         <v>23</v>
@@ -1907,19 +1898,19 @@
         <v>25</v>
       </c>
       <c r="C24" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D24" t="s">
         <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G24" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="J24" t="s">
         <v>23</v>
@@ -1936,19 +1927,19 @@
         <v>25</v>
       </c>
       <c r="C25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D25" t="s">
         <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G25" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I25" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="J25" t="s">
         <v>23</v>
@@ -1965,19 +1956,19 @@
         <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="D26" t="s">
         <v>21</v>
       </c>
       <c r="E26" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="J26" t="s">
         <v>23</v>
@@ -1994,19 +1985,19 @@
         <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D27" t="s">
         <v>21</v>
       </c>
       <c r="E27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J27" t="s">
         <v>23</v>
@@ -2023,19 +2014,19 @@
         <v>25</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
         <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G28" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I28" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J28" t="s">
         <v>23</v>
@@ -2052,19 +2043,19 @@
         <v>25</v>
       </c>
       <c r="C29" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
         <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I29" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="J29" t="s">
         <v>23</v>
@@ -2087,13 +2078,13 @@
         <v>21</v>
       </c>
       <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="G30" t="s">
+        <v>70</v>
+      </c>
+      <c r="I30" t="s">
         <v>71</v>
-      </c>
-      <c r="G30" t="s">
-        <v>72</v>
-      </c>
-      <c r="I30" t="s">
-        <v>73</v>
       </c>
       <c r="J30" t="s">
         <v>23</v>
@@ -2116,13 +2107,13 @@
         <v>21</v>
       </c>
       <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="G31" t="s">
+        <v>70</v>
+      </c>
+      <c r="I31" t="s">
         <v>71</v>
-      </c>
-      <c r="G31" t="s">
-        <v>72</v>
-      </c>
-      <c r="I31" t="s">
-        <v>73</v>
       </c>
       <c r="J31" t="s">
         <v>23</v>
@@ -2139,19 +2130,19 @@
         <v>25</v>
       </c>
       <c r="C32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D32" t="s">
         <v>21</v>
       </c>
       <c r="E32" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G32" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="I32" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="J32" t="s">
         <v>23</v>
@@ -2174,13 +2165,13 @@
         <v>21</v>
       </c>
       <c r="E33" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G33" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I33" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="J33" t="s">
         <v>23</v>
@@ -2197,19 +2188,19 @@
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D34" t="s">
         <v>21</v>
       </c>
       <c r="E34" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="G34" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I34" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="J34" t="s">
         <v>23</v>
@@ -2226,7 +2217,7 @@
         <v>25</v>
       </c>
       <c r="C35" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D35" t="s">
         <v>21</v>
@@ -2268,7 +2259,7 @@
   <sheetData>
     <row r="7" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2278,10 +2269,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06B3FAA3-4E86-4E5F-9736-210B302B7A32}">
-  <dimension ref="A1:AD29"/>
+  <dimension ref="A1:AD27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="A28" sqref="A28:XFD29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2376,28 +2367,28 @@
         <v>22</v>
       </c>
       <c r="B2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D2" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G2" t="s">
+        <v>102</v>
+      </c>
+      <c r="I2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="L2" t="s">
         <v>60</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" t="s">
-        <v>104</v>
-      </c>
-      <c r="I2" t="s">
-        <v>103</v>
-      </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
-      <c r="L2" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
@@ -2405,28 +2396,28 @@
         <v>22</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" t="s">
+        <v>70</v>
+      </c>
+      <c r="G3" t="s">
+        <v>102</v>
+      </c>
+      <c r="I3" t="s">
+        <v>126</v>
+      </c>
+      <c r="J3" t="s">
+        <v>59</v>
+      </c>
+      <c r="L3" t="s">
         <v>60</v>
-      </c>
-      <c r="C3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G3" t="s">
-        <v>104</v>
-      </c>
-      <c r="I3" t="s">
-        <v>105</v>
-      </c>
-      <c r="J3" t="s">
-        <v>61</v>
-      </c>
-      <c r="L3" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
@@ -2434,28 +2425,28 @@
         <v>22</v>
       </c>
       <c r="B4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G4" t="s">
+        <v>102</v>
+      </c>
+      <c r="I4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" t="s">
+        <v>59</v>
+      </c>
+      <c r="L4" t="s">
         <v>60</v>
-      </c>
-      <c r="C4" t="s">
-        <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" t="s">
-        <v>104</v>
-      </c>
-      <c r="I4" t="s">
-        <v>106</v>
-      </c>
-      <c r="J4" t="s">
-        <v>61</v>
-      </c>
-      <c r="L4" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
@@ -2463,28 +2454,28 @@
         <v>22</v>
       </c>
       <c r="B5" t="s">
+        <v>58</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
+      <c r="I5" t="s">
+        <v>111</v>
+      </c>
+      <c r="J5" t="s">
+        <v>59</v>
+      </c>
+      <c r="L5" t="s">
         <v>60</v>
-      </c>
-      <c r="C5" t="s">
-        <v>64</v>
-      </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" t="s">
-        <v>104</v>
-      </c>
-      <c r="I5" t="s">
-        <v>107</v>
-      </c>
-      <c r="J5" t="s">
-        <v>61</v>
-      </c>
-      <c r="L5" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.3">
@@ -2492,28 +2483,28 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" t="s">
+        <v>102</v>
+      </c>
+      <c r="I6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+      <c r="L6" t="s">
         <v>60</v>
-      </c>
-      <c r="C6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>72</v>
-      </c>
-      <c r="G6" t="s">
-        <v>104</v>
-      </c>
-      <c r="I6" t="s">
-        <v>108</v>
-      </c>
-      <c r="J6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.3">
@@ -2521,28 +2512,28 @@
         <v>22</v>
       </c>
       <c r="B7" t="s">
+        <v>58</v>
+      </c>
+      <c r="C7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" t="s">
+        <v>70</v>
+      </c>
+      <c r="G7" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" t="s">
+        <v>110</v>
+      </c>
+      <c r="J7" t="s">
+        <v>59</v>
+      </c>
+      <c r="L7" t="s">
         <v>60</v>
-      </c>
-      <c r="C7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>72</v>
-      </c>
-      <c r="G7" t="s">
-        <v>104</v>
-      </c>
-      <c r="I7" t="s">
-        <v>109</v>
-      </c>
-      <c r="J7" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.3">
@@ -2550,28 +2541,28 @@
         <v>22</v>
       </c>
       <c r="B8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G8" t="s">
+        <v>102</v>
+      </c>
+      <c r="I8" t="s">
+        <v>122</v>
+      </c>
+      <c r="J8" t="s">
+        <v>59</v>
+      </c>
+      <c r="L8" t="s">
         <v>60</v>
-      </c>
-      <c r="C8" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" t="s">
-        <v>104</v>
-      </c>
-      <c r="I8" t="s">
-        <v>110</v>
-      </c>
-      <c r="J8" t="s">
-        <v>61</v>
-      </c>
-      <c r="L8" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:30" x14ac:dyDescent="0.3">
@@ -2579,28 +2570,28 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>102</v>
+      </c>
+      <c r="I9" t="s">
+        <v>121</v>
+      </c>
+      <c r="J9" t="s">
+        <v>59</v>
+      </c>
+      <c r="L9" t="s">
         <v>60</v>
-      </c>
-      <c r="C9" t="s">
-        <v>68</v>
-      </c>
-      <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>72</v>
-      </c>
-      <c r="G9" t="s">
-        <v>104</v>
-      </c>
-      <c r="I9" t="s">
-        <v>111</v>
-      </c>
-      <c r="J9" t="s">
-        <v>61</v>
-      </c>
-      <c r="L9" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.3">
@@ -2608,28 +2599,28 @@
         <v>22</v>
       </c>
       <c r="B10" t="s">
+        <v>58</v>
+      </c>
+      <c r="C10" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>102</v>
+      </c>
+      <c r="I10" t="s">
+        <v>119</v>
+      </c>
+      <c r="J10" t="s">
+        <v>59</v>
+      </c>
+      <c r="L10" t="s">
         <v>60</v>
-      </c>
-      <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G10" t="s">
-        <v>104</v>
-      </c>
-      <c r="I10" t="s">
-        <v>105</v>
-      </c>
-      <c r="J10" t="s">
-        <v>61</v>
-      </c>
-      <c r="L10" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.3">
@@ -2637,28 +2628,28 @@
         <v>22</v>
       </c>
       <c r="B11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G11" t="s">
+        <v>102</v>
+      </c>
+      <c r="I11" t="s">
+        <v>121</v>
+      </c>
+      <c r="J11" t="s">
+        <v>59</v>
+      </c>
+      <c r="L11" t="s">
         <v>60</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G11" t="s">
-        <v>104</v>
-      </c>
-      <c r="I11" t="s">
-        <v>112</v>
-      </c>
-      <c r="J11" t="s">
-        <v>61</v>
-      </c>
-      <c r="L11" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.3">
@@ -2666,28 +2657,28 @@
         <v>22</v>
       </c>
       <c r="B12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" t="s">
+        <v>46</v>
+      </c>
+      <c r="D12" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>102</v>
+      </c>
+      <c r="I12" t="s">
+        <v>120</v>
+      </c>
+      <c r="J12" t="s">
+        <v>59</v>
+      </c>
+      <c r="L12" t="s">
         <v>60</v>
-      </c>
-      <c r="C12" t="s">
-        <v>53</v>
-      </c>
-      <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G12" t="s">
-        <v>104</v>
-      </c>
-      <c r="I12" t="s">
-        <v>113</v>
-      </c>
-      <c r="J12" t="s">
-        <v>61</v>
-      </c>
-      <c r="L12" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.3">
@@ -2695,28 +2686,28 @@
         <v>22</v>
       </c>
       <c r="B13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C13" t="s">
+        <v>43</v>
+      </c>
+      <c r="D13" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G13" t="s">
+        <v>102</v>
+      </c>
+      <c r="I13" t="s">
+        <v>117</v>
+      </c>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+      <c r="L13" t="s">
         <v>60</v>
-      </c>
-      <c r="C13" t="s">
-        <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" t="s">
-        <v>104</v>
-      </c>
-      <c r="I13" t="s">
-        <v>114</v>
-      </c>
-      <c r="J13" t="s">
-        <v>61</v>
-      </c>
-      <c r="L13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.3">
@@ -2724,7 +2715,7 @@
         <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C14" t="s">
         <v>31</v>
@@ -2733,19 +2724,19 @@
         <v>21</v>
       </c>
       <c r="E14" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.3">
@@ -2753,7 +2744,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C15" t="s">
         <v>32</v>
@@ -2762,19 +2753,19 @@
         <v>21</v>
       </c>
       <c r="E15" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="G15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="J15" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="L15" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:30" x14ac:dyDescent="0.3">
@@ -2782,28 +2773,28 @@
         <v>22</v>
       </c>
       <c r="B16" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" t="s">
+        <v>70</v>
+      </c>
+      <c r="G16" t="s">
+        <v>102</v>
+      </c>
+      <c r="I16" t="s">
+        <v>113</v>
+      </c>
+      <c r="J16" t="s">
+        <v>59</v>
+      </c>
+      <c r="L16" t="s">
         <v>60</v>
-      </c>
-      <c r="C16" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" t="s">
-        <v>72</v>
-      </c>
-      <c r="G16" t="s">
-        <v>104</v>
-      </c>
-      <c r="I16" t="s">
-        <v>117</v>
-      </c>
-      <c r="J16" t="s">
-        <v>61</v>
-      </c>
-      <c r="L16" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.3">
@@ -2811,28 +2802,28 @@
         <v>22</v>
       </c>
       <c r="B17" t="s">
+        <v>58</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" t="s">
+        <v>70</v>
+      </c>
+      <c r="G17" t="s">
+        <v>102</v>
+      </c>
+      <c r="I17" t="s">
+        <v>115</v>
+      </c>
+      <c r="J17" t="s">
+        <v>59</v>
+      </c>
+      <c r="L17" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>69</v>
-      </c>
-      <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>72</v>
-      </c>
-      <c r="G17" t="s">
-        <v>104</v>
-      </c>
-      <c r="I17" t="s">
-        <v>118</v>
-      </c>
-      <c r="J17" t="s">
-        <v>61</v>
-      </c>
-      <c r="L17" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
@@ -2840,28 +2831,28 @@
         <v>22</v>
       </c>
       <c r="B18" t="s">
+        <v>58</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>70</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
+      </c>
+      <c r="I18" t="s">
+        <v>114</v>
+      </c>
+      <c r="J18" t="s">
+        <v>59</v>
+      </c>
+      <c r="L18" t="s">
         <v>60</v>
-      </c>
-      <c r="C18" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>72</v>
-      </c>
-      <c r="G18" t="s">
-        <v>104</v>
-      </c>
-      <c r="I18" t="s">
-        <v>119</v>
-      </c>
-      <c r="J18" t="s">
-        <v>61</v>
-      </c>
-      <c r="L18" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
@@ -2869,28 +2860,28 @@
         <v>22</v>
       </c>
       <c r="B19" t="s">
+        <v>58</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" t="s">
+        <v>102</v>
+      </c>
+      <c r="I19" t="s">
+        <v>101</v>
+      </c>
+      <c r="J19" t="s">
+        <v>59</v>
+      </c>
+      <c r="L19" t="s">
         <v>60</v>
-      </c>
-      <c r="C19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>72</v>
-      </c>
-      <c r="G19" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" t="s">
-        <v>120</v>
-      </c>
-      <c r="J19" t="s">
-        <v>61</v>
-      </c>
-      <c r="L19" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
@@ -2898,28 +2889,28 @@
         <v>22</v>
       </c>
       <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>26</v>
+      </c>
+      <c r="D20" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" t="s">
+        <v>70</v>
+      </c>
+      <c r="G20" t="s">
+        <v>102</v>
+      </c>
+      <c r="I20" t="s">
+        <v>103</v>
+      </c>
+      <c r="J20" t="s">
+        <v>59</v>
+      </c>
+      <c r="L20" t="s">
         <v>60</v>
-      </c>
-      <c r="C20" t="s">
-        <v>34</v>
-      </c>
-      <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>72</v>
-      </c>
-      <c r="G20" t="s">
-        <v>104</v>
-      </c>
-      <c r="I20" t="s">
-        <v>121</v>
-      </c>
-      <c r="J20" t="s">
-        <v>61</v>
-      </c>
-      <c r="L20" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
@@ -2927,28 +2918,28 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C21" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" t="s">
+        <v>102</v>
+      </c>
+      <c r="I21" t="s">
+        <v>112</v>
+      </c>
+      <c r="J21" t="s">
+        <v>59</v>
+      </c>
+      <c r="L21" t="s">
         <v>60</v>
-      </c>
-      <c r="C21" t="s">
-        <v>35</v>
-      </c>
-      <c r="D21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>72</v>
-      </c>
-      <c r="G21" t="s">
-        <v>104</v>
-      </c>
-      <c r="I21" t="s">
-        <v>122</v>
-      </c>
-      <c r="J21" t="s">
-        <v>61</v>
-      </c>
-      <c r="L21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
@@ -2956,28 +2947,28 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" t="s">
+        <v>66</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>70</v>
+      </c>
+      <c r="G22" t="s">
+        <v>102</v>
+      </c>
+      <c r="I22" t="s">
+        <v>109</v>
+      </c>
+      <c r="J22" t="s">
+        <v>59</v>
+      </c>
+      <c r="L22" t="s">
         <v>60</v>
-      </c>
-      <c r="C22" t="s">
-        <v>48</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>72</v>
-      </c>
-      <c r="G22" t="s">
-        <v>104</v>
-      </c>
-      <c r="I22" t="s">
-        <v>123</v>
-      </c>
-      <c r="J22" t="s">
-        <v>61</v>
-      </c>
-      <c r="L22" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
@@ -2985,28 +2976,28 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" t="s">
+        <v>65</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" t="s">
+        <v>102</v>
+      </c>
+      <c r="I23" t="s">
+        <v>108</v>
+      </c>
+      <c r="J23" t="s">
+        <v>59</v>
+      </c>
+      <c r="L23" t="s">
         <v>60</v>
-      </c>
-      <c r="C23" t="s">
-        <v>36</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>72</v>
-      </c>
-      <c r="G23" t="s">
-        <v>104</v>
-      </c>
-      <c r="I23" t="s">
-        <v>124</v>
-      </c>
-      <c r="J23" t="s">
-        <v>61</v>
-      </c>
-      <c r="L23" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
@@ -3014,28 +3005,28 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
+        <v>58</v>
+      </c>
+      <c r="C24" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" t="s">
+        <v>70</v>
+      </c>
+      <c r="G24" t="s">
+        <v>102</v>
+      </c>
+      <c r="I24" t="s">
+        <v>107</v>
+      </c>
+      <c r="J24" t="s">
+        <v>59</v>
+      </c>
+      <c r="L24" t="s">
         <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>37</v>
-      </c>
-      <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>72</v>
-      </c>
-      <c r="G24" t="s">
-        <v>104</v>
-      </c>
-      <c r="I24" t="s">
-        <v>125</v>
-      </c>
-      <c r="J24" t="s">
-        <v>61</v>
-      </c>
-      <c r="L24" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.3">
@@ -3043,28 +3034,28 @@
         <v>22</v>
       </c>
       <c r="B25" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" t="s">
+        <v>21</v>
+      </c>
+      <c r="E25" t="s">
+        <v>70</v>
+      </c>
+      <c r="G25" t="s">
+        <v>102</v>
+      </c>
+      <c r="I25" t="s">
+        <v>106</v>
+      </c>
+      <c r="J25" t="s">
+        <v>59</v>
+      </c>
+      <c r="L25" t="s">
         <v>60</v>
-      </c>
-      <c r="C25" t="s">
-        <v>51</v>
-      </c>
-      <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>72</v>
-      </c>
-      <c r="G25" t="s">
-        <v>104</v>
-      </c>
-      <c r="I25" t="s">
-        <v>126</v>
-      </c>
-      <c r="J25" t="s">
-        <v>61</v>
-      </c>
-      <c r="L25" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
@@ -3072,28 +3063,28 @@
         <v>22</v>
       </c>
       <c r="B26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C26" t="s">
+        <v>62</v>
+      </c>
+      <c r="D26" t="s">
+        <v>21</v>
+      </c>
+      <c r="E26" t="s">
+        <v>69</v>
+      </c>
+      <c r="G26" t="s">
+        <v>102</v>
+      </c>
+      <c r="I26" t="s">
+        <v>105</v>
+      </c>
+      <c r="J26" t="s">
+        <v>59</v>
+      </c>
+      <c r="L26" t="s">
         <v>60</v>
-      </c>
-      <c r="C26" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" t="s">
-        <v>72</v>
-      </c>
-      <c r="G26" t="s">
-        <v>104</v>
-      </c>
-      <c r="I26" t="s">
-        <v>124</v>
-      </c>
-      <c r="J26" t="s">
-        <v>61</v>
-      </c>
-      <c r="L26" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
@@ -3101,89 +3092,34 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" t="s">
+        <v>61</v>
+      </c>
+      <c r="D27" t="s">
+        <v>21</v>
+      </c>
+      <c r="E27" t="s">
+        <v>70</v>
+      </c>
+      <c r="G27" t="s">
+        <v>102</v>
+      </c>
+      <c r="I27" t="s">
+        <v>104</v>
+      </c>
+      <c r="J27" t="s">
+        <v>59</v>
+      </c>
+      <c r="L27" t="s">
         <v>60</v>
       </c>
-      <c r="C27" t="s">
-        <v>39</v>
-      </c>
-      <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" t="s">
-        <v>104</v>
-      </c>
-      <c r="I27" t="s">
-        <v>127</v>
-      </c>
-      <c r="J27" t="s">
-        <v>61</v>
-      </c>
-      <c r="L27" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" t="s">
-        <v>54</v>
-      </c>
-      <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" t="s">
-        <v>72</v>
-      </c>
-      <c r="G28" t="s">
-        <v>104</v>
-      </c>
-      <c r="I28" t="s">
-        <v>128</v>
-      </c>
-      <c r="J28" t="s">
-        <v>61</v>
-      </c>
-      <c r="L28" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" t="s">
-        <v>72</v>
-      </c>
-      <c r="G29" t="s">
-        <v>104</v>
-      </c>
-      <c r="I29" t="s">
-        <v>129</v>
-      </c>
-      <c r="J29" t="s">
-        <v>61</v>
-      </c>
-      <c r="L29" t="s">
-        <v>62</v>
-      </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U29">
+    <sortCondition ref="C1"/>
+  </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
   <conditionalFormatting sqref="D1">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
@@ -3210,12 +3146,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
   </sheetData>
@@ -3235,7 +3171,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating excel and code
</commit_message>
<xml_diff>
--- a/data/T29R09_data.xlsx
+++ b/data/T29R09_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Ecology\Student_folders_&amp;_files\Kara 2020\GLO\Sage_GLO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EDD7494-7AF5-4C3A-92CC-FE1AC19D8A87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B4BC0B-1D76-44BF-A89A-779177987834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
   </bookViews>
@@ -3253,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C2F317-3C47-4C49-B514-2E7FE2EC3A02}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C63" sqref="C63:C73"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C53" sqref="C53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3293,7 +3293,7 @@
         <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -3414,7 +3414,7 @@
         <v>163</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -3546,7 +3546,7 @@
         <v>157</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -3843,7 +3843,7 @@
         <v>140</v>
       </c>
       <c r="C53" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
@@ -3953,7 +3953,7 @@
         <v>135</v>
       </c>
       <c r="C63" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -4052,7 +4052,7 @@
         <v>131</v>
       </c>
       <c r="C72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updating for final figures
</commit_message>
<xml_diff>
--- a/data/T29R09_data.xlsx
+++ b/data/T29R09_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Ecology\Student_folders_&amp;_files\Kara 2020\GLO\Sage_GLO\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42B4BC0B-1D76-44BF-A89A-779177987834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68CBD63-6EDD-49F0-9704-3AAB526B5A94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{57E6658A-972A-45D4-998A-4D33D82BBA9F}"/>
   </bookViews>
   <sheets>
     <sheet name="1880Survey" sheetId="1" r:id="rId1"/>
@@ -116,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{00EE9CFC-0C91-4B13-A07E-4D9F41D9AD05}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00EE9CFC-0C91-4B13-A07E-4D9F41D9AD05}">
       <text>
         <r>
           <rPr>
@@ -132,7 +132,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{88021CBC-E3A0-4E61-8ACF-7F8D0D2FB89A}">
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{88021CBC-E3A0-4E61-8ACF-7F8D0D2FB89A}">
       <text>
         <r>
           <rPr>
@@ -148,7 +148,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{DBF13A1A-DCCD-4C3F-93F4-2235033C2C6A}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{DBF13A1A-DCCD-4C3F-93F4-2235033C2C6A}">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{A5C315F7-7859-4D45-8D87-1AE4CD613A44}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{A5C315F7-7859-4D45-8D87-1AE4CD613A44}">
       <text>
         <r>
           <rPr>
@@ -178,7 +178,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U1" authorId="0" shapeId="0" xr:uid="{6D09D289-2A09-4F16-AE6B-564174ABF53A}">
+    <comment ref="T1" authorId="0" shapeId="0" xr:uid="{6D09D289-2A09-4F16-AE6B-564174ABF53A}">
       <text>
         <r>
           <rPr>
@@ -1278,10 +1278,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A5C64BF-EBB4-4133-9976-AA11B41391F4}">
-  <dimension ref="A1:AD35"/>
+  <dimension ref="A1:AC35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35:XFD39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1289,14 +1289,14 @@
     <col min="1" max="1" width="15.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.140625" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="6" max="6" width="3.42578125" customWidth="1"/>
-    <col min="9" max="9" width="60.28515625" customWidth="1"/>
-    <col min="10" max="10" width="12.140625" customWidth="1"/>
-    <col min="11" max="11" width="18" customWidth="1"/>
-    <col min="12" max="12" width="22.28515625" customWidth="1"/>
+    <col min="5" max="5" width="3.42578125" customWidth="1"/>
+    <col min="8" max="8" width="60.28515625" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="18" customWidth="1"/>
+    <col min="11" max="11" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1306,59 +1306,59 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="2" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
@@ -1368,9 +1368,8 @@
       <c r="AA1" s="4"/>
       <c r="AB1" s="4"/>
       <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-    </row>
-    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -1381,25 +1380,25 @@
         <v>37</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
         <v>73</v>
       </c>
+      <c r="H2" t="s">
+        <v>82</v>
+      </c>
       <c r="I2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J2" t="s">
         <v>23</v>
       </c>
-      <c r="L2" t="s">
+      <c r="K2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -1410,25 +1409,25 @@
         <v>38</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F3" t="s">
         <v>73</v>
       </c>
+      <c r="H3" t="s">
+        <v>83</v>
+      </c>
       <c r="I3" t="s">
-        <v>83</v>
-      </c>
-      <c r="J3" t="s">
         <v>23</v>
       </c>
-      <c r="L3" t="s">
+      <c r="K3" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -1439,25 +1438,25 @@
         <v>52</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F4" t="s">
+        <v>70</v>
+      </c>
+      <c r="H4" t="s">
+        <v>96</v>
       </c>
       <c r="I4" t="s">
-        <v>96</v>
-      </c>
-      <c r="J4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -1468,25 +1467,25 @@
         <v>55</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
-      <c r="G5" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="H5" t="s">
+        <v>74</v>
       </c>
       <c r="I5" t="s">
-        <v>74</v>
-      </c>
-      <c r="J5" t="s">
         <v>23</v>
       </c>
-      <c r="L5" t="s">
+      <c r="K5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1497,25 +1496,25 @@
         <v>53</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" t="s">
-        <v>69</v>
-      </c>
-      <c r="G6" t="s">
+        <v>69</v>
+      </c>
+      <c r="F6" t="s">
         <v>73</v>
       </c>
+      <c r="H6" t="s">
+        <v>72</v>
+      </c>
       <c r="I6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J6" t="s">
         <v>23</v>
       </c>
-      <c r="L6" t="s">
+      <c r="K6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -1526,25 +1525,25 @@
         <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" t="s">
-        <v>69</v>
-      </c>
-      <c r="G7" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
+        <v>98</v>
       </c>
       <c r="I7" t="s">
-        <v>98</v>
-      </c>
-      <c r="J7" t="s">
         <v>23</v>
       </c>
-      <c r="L7" t="s">
+      <c r="K7" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -1555,25 +1554,25 @@
         <v>56</v>
       </c>
       <c r="D8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" t="s">
+        <v>69</v>
+      </c>
+      <c r="F8" t="s">
         <v>73</v>
       </c>
+      <c r="H8" t="s">
+        <v>99</v>
+      </c>
       <c r="I8" t="s">
-        <v>99</v>
-      </c>
-      <c r="J8" t="s">
         <v>23</v>
       </c>
-      <c r="L8" t="s">
+      <c r="K8" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -1584,25 +1583,25 @@
         <v>50</v>
       </c>
       <c r="D9" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" t="s">
-        <v>69</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>95</v>
       </c>
       <c r="I9" t="s">
-        <v>95</v>
-      </c>
-      <c r="J9" t="s">
         <v>23</v>
       </c>
-      <c r="L9" t="s">
+      <c r="K9" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -1613,25 +1612,25 @@
         <v>97</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" t="s">
-        <v>69</v>
-      </c>
-      <c r="G10" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" t="s">
+        <v>74</v>
       </c>
       <c r="I10" t="s">
-        <v>74</v>
-      </c>
-      <c r="J10" t="s">
         <v>23</v>
       </c>
-      <c r="L10" t="s">
+      <c r="K10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U10" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1642,25 +1641,25 @@
         <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" t="s">
-        <v>69</v>
-      </c>
-      <c r="G11" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F11" t="s">
+        <v>70</v>
+      </c>
+      <c r="H11" t="s">
+        <v>94</v>
       </c>
       <c r="I11" t="s">
-        <v>94</v>
-      </c>
-      <c r="J11" t="s">
         <v>23</v>
       </c>
-      <c r="L11" t="s">
+      <c r="K11" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1671,25 +1670,25 @@
         <v>51</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
+        <v>74</v>
       </c>
       <c r="I12" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" t="s">
         <v>23</v>
       </c>
-      <c r="L12" t="s">
+      <c r="K12" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
@@ -1700,25 +1699,25 @@
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" t="s">
-        <v>69</v>
-      </c>
-      <c r="G13" t="s">
+        <v>69</v>
+      </c>
+      <c r="F13" t="s">
         <v>73</v>
       </c>
+      <c r="H13" t="s">
+        <v>80</v>
+      </c>
       <c r="I13" t="s">
-        <v>80</v>
-      </c>
-      <c r="J13" t="s">
         <v>23</v>
       </c>
-      <c r="L13" t="s">
+      <c r="K13" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="14" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U13" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>22</v>
       </c>
@@ -1729,25 +1728,25 @@
         <v>36</v>
       </c>
       <c r="D14" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" t="s">
-        <v>69</v>
-      </c>
-      <c r="G14" t="s">
+        <v>69</v>
+      </c>
+      <c r="F14" t="s">
         <v>73</v>
       </c>
+      <c r="H14" t="s">
+        <v>81</v>
+      </c>
       <c r="I14" t="s">
-        <v>81</v>
-      </c>
-      <c r="J14" t="s">
         <v>23</v>
       </c>
-      <c r="L14" t="s">
+      <c r="K14" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="15" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1758,25 +1757,25 @@
         <v>33</v>
       </c>
       <c r="D15" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" t="s">
-        <v>69</v>
-      </c>
-      <c r="G15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" t="s">
         <v>73</v>
       </c>
+      <c r="H15" t="s">
+        <v>79</v>
+      </c>
       <c r="I15" t="s">
-        <v>79</v>
-      </c>
-      <c r="J15" t="s">
         <v>23</v>
       </c>
-      <c r="L15" t="s">
+      <c r="K15" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="U15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -1787,25 +1786,25 @@
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" t="s">
         <v>73</v>
       </c>
+      <c r="H16" t="s">
+        <v>80</v>
+      </c>
       <c r="I16" t="s">
-        <v>80</v>
-      </c>
-      <c r="J16" t="s">
         <v>23</v>
       </c>
-      <c r="L16" t="s">
+      <c r="K16" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1816,25 +1815,25 @@
         <v>46</v>
       </c>
       <c r="D17" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" t="s">
-        <v>69</v>
-      </c>
-      <c r="G17" t="s">
+        <v>69</v>
+      </c>
+      <c r="F17" t="s">
         <v>73</v>
       </c>
+      <c r="H17" t="s">
+        <v>88</v>
+      </c>
       <c r="I17" t="s">
-        <v>88</v>
-      </c>
-      <c r="J17" t="s">
         <v>23</v>
       </c>
-      <c r="L17" t="s">
+      <c r="K17" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U17" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -1845,25 +1844,25 @@
         <v>48</v>
       </c>
       <c r="D18" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" t="s">
-        <v>69</v>
-      </c>
-      <c r="G18" t="s">
+        <v>69</v>
+      </c>
+      <c r="F18" t="s">
         <v>92</v>
       </c>
+      <c r="H18" t="s">
+        <v>91</v>
+      </c>
       <c r="I18" t="s">
-        <v>91</v>
-      </c>
-      <c r="J18" t="s">
         <v>23</v>
       </c>
-      <c r="L18" t="s">
+      <c r="K18" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U18" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>22</v>
       </c>
@@ -1874,25 +1873,25 @@
         <v>47</v>
       </c>
       <c r="D19" t="s">
-        <v>21</v>
-      </c>
-      <c r="E19" t="s">
-        <v>69</v>
-      </c>
-      <c r="G19" t="s">
+        <v>69</v>
+      </c>
+      <c r="F19" t="s">
         <v>73</v>
       </c>
+      <c r="H19" t="s">
+        <v>90</v>
+      </c>
       <c r="I19" t="s">
-        <v>90</v>
-      </c>
-      <c r="J19" t="s">
         <v>23</v>
       </c>
-      <c r="L19" t="s">
+      <c r="K19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U19" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1903,25 +1902,25 @@
         <v>44</v>
       </c>
       <c r="D20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E20" t="s">
-        <v>69</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F20" t="s">
+        <v>70</v>
+      </c>
+      <c r="H20" t="s">
+        <v>89</v>
       </c>
       <c r="I20" t="s">
-        <v>89</v>
-      </c>
-      <c r="J20" t="s">
         <v>23</v>
       </c>
-      <c r="L20" t="s">
+      <c r="K20" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -1932,25 +1931,25 @@
         <v>43</v>
       </c>
       <c r="D21" t="s">
-        <v>21</v>
-      </c>
-      <c r="E21" t="s">
-        <v>70</v>
-      </c>
-      <c r="G21" t="s">
-        <v>70</v>
+        <v>70</v>
+      </c>
+      <c r="F21" t="s">
+        <v>70</v>
+      </c>
+      <c r="H21" t="s">
+        <v>87</v>
       </c>
       <c r="I21" t="s">
-        <v>87</v>
-      </c>
-      <c r="J21" t="s">
         <v>23</v>
       </c>
-      <c r="L21" t="s">
+      <c r="K21" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U21" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>22</v>
       </c>
@@ -1961,25 +1960,25 @@
         <v>45</v>
       </c>
       <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>69</v>
-      </c>
-      <c r="G22" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" t="s">
         <v>73</v>
       </c>
+      <c r="H22" t="s">
+        <v>88</v>
+      </c>
       <c r="I22" t="s">
-        <v>88</v>
-      </c>
-      <c r="J22" t="s">
         <v>23</v>
       </c>
-      <c r="L22" t="s">
+      <c r="K22" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1990,25 +1989,25 @@
         <v>31</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>69</v>
-      </c>
-      <c r="G23" t="s">
-        <v>69</v>
+        <v>69</v>
+      </c>
+      <c r="F23" t="s">
+        <v>69</v>
+      </c>
+      <c r="H23" t="s">
+        <v>77</v>
       </c>
       <c r="I23" t="s">
-        <v>77</v>
-      </c>
-      <c r="J23" t="s">
         <v>23</v>
       </c>
-      <c r="L23" t="s">
+      <c r="K23" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2019,25 +2018,25 @@
         <v>32</v>
       </c>
       <c r="D24" t="s">
-        <v>21</v>
-      </c>
-      <c r="E24" t="s">
-        <v>69</v>
-      </c>
-      <c r="G24" t="s">
+        <v>69</v>
+      </c>
+      <c r="F24" t="s">
         <v>73</v>
       </c>
+      <c r="H24" t="s">
+        <v>78</v>
+      </c>
       <c r="I24" t="s">
-        <v>78</v>
-      </c>
-      <c r="J24" t="s">
         <v>23</v>
       </c>
-      <c r="L24" t="s">
+      <c r="K24" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U24" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -2048,25 +2047,25 @@
         <v>30</v>
       </c>
       <c r="D25" t="s">
-        <v>21</v>
-      </c>
-      <c r="E25" t="s">
-        <v>69</v>
-      </c>
-      <c r="G25" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F25" t="s">
+        <v>70</v>
+      </c>
+      <c r="H25" t="s">
+        <v>75</v>
       </c>
       <c r="I25" t="s">
-        <v>75</v>
-      </c>
-      <c r="J25" t="s">
         <v>23</v>
       </c>
-      <c r="L25" t="s">
+      <c r="K25" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U25" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2077,25 +2076,25 @@
         <v>67</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
-      </c>
-      <c r="E26" t="s">
-        <v>69</v>
-      </c>
-      <c r="G26" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F26" t="s">
+        <v>70</v>
+      </c>
+      <c r="H26" t="s">
+        <v>76</v>
       </c>
       <c r="I26" t="s">
-        <v>76</v>
-      </c>
-      <c r="J26" t="s">
         <v>23</v>
       </c>
-      <c r="L26" t="s">
+      <c r="K26" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U26" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -2106,25 +2105,25 @@
         <v>40</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
-      </c>
-      <c r="E27" t="s">
-        <v>69</v>
-      </c>
-      <c r="G27" t="s">
+        <v>69</v>
+      </c>
+      <c r="F27" t="s">
         <v>73</v>
       </c>
+      <c r="H27" t="s">
+        <v>85</v>
+      </c>
       <c r="I27" t="s">
-        <v>85</v>
-      </c>
-      <c r="J27" t="s">
         <v>23</v>
       </c>
-      <c r="L27" t="s">
+      <c r="K27" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -2135,25 +2134,25 @@
         <v>41</v>
       </c>
       <c r="D28" t="s">
-        <v>21</v>
-      </c>
-      <c r="E28" t="s">
-        <v>69</v>
-      </c>
-      <c r="G28" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F28" t="s">
+        <v>70</v>
+      </c>
+      <c r="H28" t="s">
+        <v>74</v>
       </c>
       <c r="I28" t="s">
-        <v>74</v>
-      </c>
-      <c r="J28" t="s">
         <v>23</v>
       </c>
-      <c r="L28" t="s">
+      <c r="K28" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>22</v>
       </c>
@@ -2164,25 +2163,25 @@
         <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>21</v>
-      </c>
-      <c r="E29" t="s">
-        <v>69</v>
-      </c>
-      <c r="G29" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>70</v>
+      </c>
+      <c r="H29" t="s">
+        <v>86</v>
       </c>
       <c r="I29" t="s">
-        <v>86</v>
-      </c>
-      <c r="J29" t="s">
         <v>23</v>
       </c>
-      <c r="L29" t="s">
+      <c r="K29" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -2193,25 +2192,25 @@
         <v>28</v>
       </c>
       <c r="D30" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" t="s">
-        <v>69</v>
-      </c>
-      <c r="G30" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
+        <v>70</v>
+      </c>
+      <c r="H30" t="s">
+        <v>71</v>
       </c>
       <c r="I30" t="s">
-        <v>71</v>
-      </c>
-      <c r="J30" t="s">
         <v>23</v>
       </c>
-      <c r="L30" t="s">
+      <c r="K30" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U30" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -2222,25 +2221,25 @@
         <v>27</v>
       </c>
       <c r="D31" t="s">
-        <v>21</v>
-      </c>
-      <c r="E31" t="s">
-        <v>69</v>
-      </c>
-      <c r="G31" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
+        <v>70</v>
+      </c>
+      <c r="H31" t="s">
+        <v>71</v>
       </c>
       <c r="I31" t="s">
-        <v>71</v>
-      </c>
-      <c r="J31" t="s">
         <v>23</v>
       </c>
-      <c r="L31" t="s">
+      <c r="K31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -2251,25 +2250,25 @@
         <v>39</v>
       </c>
       <c r="D32" t="s">
-        <v>21</v>
-      </c>
-      <c r="E32" t="s">
-        <v>69</v>
-      </c>
-      <c r="G32" t="s">
+        <v>69</v>
+      </c>
+      <c r="F32" t="s">
         <v>73</v>
       </c>
+      <c r="H32" t="s">
+        <v>85</v>
+      </c>
       <c r="I32" t="s">
-        <v>85</v>
-      </c>
-      <c r="J32" t="s">
         <v>23</v>
       </c>
-      <c r="L32" t="s">
+      <c r="K32" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U32" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -2280,25 +2279,25 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>21</v>
-      </c>
-      <c r="E33" t="s">
-        <v>69</v>
-      </c>
-      <c r="G33" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F33" t="s">
+        <v>70</v>
+      </c>
+      <c r="H33" t="s">
+        <v>68</v>
       </c>
       <c r="I33" t="s">
-        <v>68</v>
-      </c>
-      <c r="J33" t="s">
         <v>23</v>
       </c>
-      <c r="L33" t="s">
+      <c r="K33" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -2309,25 +2308,25 @@
         <v>29</v>
       </c>
       <c r="D34" t="s">
-        <v>21</v>
-      </c>
-      <c r="E34" t="s">
-        <v>69</v>
-      </c>
-      <c r="G34" t="s">
-        <v>70</v>
+        <v>69</v>
+      </c>
+      <c r="F34" t="s">
+        <v>70</v>
+      </c>
+      <c r="H34" t="s">
+        <v>74</v>
       </c>
       <c r="I34" t="s">
-        <v>74</v>
-      </c>
-      <c r="J34" t="s">
         <v>23</v>
       </c>
-      <c r="L34" t="s">
+      <c r="K34" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="U34" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>22</v>
       </c>
@@ -2337,24 +2336,24 @@
       <c r="C35" t="s">
         <v>57</v>
       </c>
-      <c r="D35" t="s">
-        <v>21</v>
-      </c>
-      <c r="J35" t="s">
+      <c r="I35" t="s">
         <v>23</v>
       </c>
-      <c r="L35" t="s">
+      <c r="K35" t="s">
         <v>24</v>
       </c>
+      <c r="U35" t="s">
+        <v>21</v>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U35">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T35">
     <sortCondition ref="C1"/>
   </sortState>
   <phoneticPr fontId="5" type="noConversion"/>
-  <conditionalFormatting sqref="D1">
+  <conditionalFormatting sqref="U1">
     <cfRule type="notContainsBlanks" dxfId="1" priority="1">
-      <formula>LEN(TRIM(D1))&gt;0</formula>
+      <formula>LEN(TRIM(U1))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3253,8 +3252,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41C2F317-3C47-4C49-B514-2E7FE2EC3A02}">
   <dimension ref="A1:C73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C53" sqref="C53"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>